<commit_message>
Fixing broken links, hiding solutions that aren't posted yet
</commit_message>
<xml_diff>
--- a/files/schedule_modules.xlsx
+++ b/files/schedule_modules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu-my.sharepoint.com/personal/cooperstone_1_osu_edu/Documents/BuckeyeBox Data/JLC_Files/OSU/teaching/data-viz/dataviz-site/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu-my.sharepoint.com/personal/cooperstone_1_osu_edu/Documents/BuckeyeBox Data/JLC_Files/OSU/teaching/data-viz/rdataviz/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{7C40CE6C-DF63-484C-A234-8A007B7633E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2402478F-0A11-9A46-B13F-0C7B57C2BA50}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{7C40CE6C-DF63-484C-A234-8A007B7633E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F75A90A-1834-D546-A787-FE59258F99FE}"/>
   <bookViews>
-    <workbookView xWindow="17520" yWindow="5740" windowWidth="28800" windowHeight="16360" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
+    <workbookView xWindow="5540" yWindow="6340" windowWidth="28800" windowHeight="16360" activeTab="2" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="33">
   <si>
     <t>Principles of data visualization</t>
   </si>
@@ -117,13 +117,25 @@
     <t>Due Date</t>
   </si>
   <si>
-    <t>1: Good and bad visualizations</t>
-  </si>
-  <si>
-    <t>2: Coding Fundamentals</t>
-  </si>
-  <si>
-    <t>3: Data Exploration</t>
+    <t>Assignment</t>
+  </si>
+  <si>
+    <t>Module 1: Good and bad visualizations</t>
+  </si>
+  <si>
+    <t>Module 2: Coding Fundamentals</t>
+  </si>
+  <si>
+    <t>Module 3: Data Exploration</t>
+  </si>
+  <si>
+    <t>Module 4: Putting it together</t>
+  </si>
+  <si>
+    <t>Capstone plan</t>
+  </si>
+  <si>
+    <t>Capstone</t>
   </si>
 </sst>
 </file>
@@ -479,7 +491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F342C0D-B564-AC4C-B9F2-1430BA1BF96D}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -888,10 +900,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48504950-6619-024D-BFE6-3D795EC0E695}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -901,7 +913,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>25</v>
@@ -909,7 +921,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2">
         <v>45166</v>
@@ -917,7 +929,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2">
         <v>45202</v>
@@ -925,7 +937,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2">
         <v>45230</v>
@@ -933,9 +945,25 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2">
+        <v>45265</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2">
         <v>45265</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating for autumn 2024
</commit_message>
<xml_diff>
--- a/files/schedule_modules.xlsx
+++ b/files/schedule_modules.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu-my.sharepoint.com/personal/cooperstone_1_osu_edu/Documents/BuckeyeBox Data/JLC_Files/OSU/teaching/data-viz/rdataviz/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{7C40CE6C-DF63-484C-A234-8A007B7633E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F75A90A-1834-D546-A787-FE59258F99FE}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{7C40CE6C-DF63-484C-A234-8A007B7633E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DE9FDC5-32D3-3348-902C-1E098ACB4C55}"/>
   <bookViews>
-    <workbookView xWindow="5540" yWindow="6340" windowWidth="28800" windowHeight="16360" activeTab="2" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
+    <workbookView xWindow="13060" yWindow="3680" windowWidth="28800" windowHeight="16360" activeTab="2" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="2" r:id="rId1"/>
-    <sheet name="Schedule_date" sheetId="3" r:id="rId2"/>
-    <sheet name="module_due_dates" sheetId="4" r:id="rId3"/>
+    <sheet name="Schedule_date_2024" sheetId="5" r:id="rId2"/>
+    <sheet name="module_due_dates_2024" sheetId="6" r:id="rId3"/>
+    <sheet name="Schedule_date_2023" sheetId="3" r:id="rId4"/>
+    <sheet name="module_due_dates_2023" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,6 +32,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="41">
   <si>
     <t>Principles of data visualization</t>
   </si>
@@ -136,6 +139,30 @@
   </si>
   <si>
     <t>Capstone</t>
+  </si>
+  <si>
+    <t>Reflections</t>
+  </si>
+  <si>
+    <t>1 week after each class</t>
+  </si>
+  <si>
+    <t>Monday, August 26, 2024</t>
+  </si>
+  <si>
+    <t>Tuesday, October 1, 2024</t>
+  </si>
+  <si>
+    <t>Tuesday, December 3, 2024</t>
+  </si>
+  <si>
+    <t>Tuesday, November 5, 2024</t>
+  </si>
+  <si>
+    <t>Friday, December 6, 2024</t>
+  </si>
+  <si>
+    <t>Tuesday, October 29, 2024</t>
   </si>
 </sst>
 </file>
@@ -193,9 +220,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -233,7 +260,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -339,7 +366,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -481,7 +508,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -693,11 +720,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AC0B77-377C-2E43-B142-D9BC271E0496}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E7002E-0E54-7A4A-93D0-B7490C5E682B}">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C17"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -719,7 +746,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>45160</v>
+        <v>45524</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -730,7 +757,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>45167</v>
+        <v>45531</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -741,7 +768,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>45174</v>
+        <v>45538</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -752,7 +779,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>45181</v>
+        <v>45545</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -763,7 +790,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>45188</v>
+        <v>45552</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
@@ -774,7 +801,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>45195</v>
+        <v>45559</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
@@ -785,7 +812,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>45202</v>
+        <v>45566</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -796,7 +823,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>45209</v>
+        <v>45573</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -807,7 +834,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>45216</v>
+        <v>45580</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -818,7 +845,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>45223</v>
+        <v>45587</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
@@ -829,7 +856,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>45230</v>
+        <v>45594</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -840,7 +867,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>45237</v>
+        <v>45601</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -851,7 +878,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>45244</v>
+        <v>45608</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -862,29 +889,29 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>45251</v>
+        <v>45615</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>45258</v>
+        <v>45622</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>45265</v>
+        <v>45629</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
@@ -899,10 +926,300 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB6305A-7A3D-E944-958B-BA084CA13D72}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AC0B77-377C-2E43-B142-D9BC271E0496}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>45160</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>45167</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>45174</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>45181</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>45188</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>45195</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>45202</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>45209</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>45216</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>45223</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>45230</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>45237</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>45244</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>45251</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>45265</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48504950-6619-024D-BFE6-3D795EC0E695}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updating syllabus, lecture 1 and 2
</commit_message>
<xml_diff>
--- a/files/schedule_modules.xlsx
+++ b/files/schedule_modules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu-my.sharepoint.com/personal/cooperstone_1_osu_edu/Documents/BuckeyeBox Data/JLC_Files/OSU/teaching/data-viz/rdataviz/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{7C40CE6C-DF63-484C-A234-8A007B7633E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DE9FDC5-32D3-3348-902C-1E098ACB4C55}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="13_ncr:1_{7C40CE6C-DF63-484C-A234-8A007B7633E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DADFFC60-5773-D145-B141-C181D957E330}"/>
   <bookViews>
-    <workbookView xWindow="13060" yWindow="3680" windowWidth="28800" windowHeight="16360" activeTab="2" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
+    <workbookView xWindow="13060" yWindow="3680" windowWidth="28800" windowHeight="16360" activeTab="1" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="2" r:id="rId1"/>
@@ -169,6 +169,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -198,10 +201,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,19 +725,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E7002E-0E54-7A4A-93D0-B7490C5E682B}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -744,8 +748,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
         <v>45524</v>
       </c>
       <c r="B2" t="s">
@@ -754,9 +758,10 @@
       <c r="C2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>45531</v>
       </c>
       <c r="B3" t="s">
@@ -765,9 +770,10 @@
       <c r="C3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>45538</v>
       </c>
       <c r="B4" t="s">
@@ -776,9 +782,10 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>45545</v>
       </c>
       <c r="B5" t="s">
@@ -787,9 +794,10 @@
       <c r="C5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>45552</v>
       </c>
       <c r="B6" t="s">
@@ -798,9 +806,10 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>45559</v>
       </c>
       <c r="B7" t="s">
@@ -809,9 +818,10 @@
       <c r="C7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
         <v>45566</v>
       </c>
       <c r="B8" t="s">
@@ -820,9 +830,10 @@
       <c r="C8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
         <v>45573</v>
       </c>
       <c r="B9" t="s">
@@ -831,9 +842,10 @@
       <c r="C9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
         <v>45580</v>
       </c>
       <c r="B10" t="s">
@@ -842,9 +854,10 @@
       <c r="C10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
         <v>45587</v>
       </c>
       <c r="B11" t="s">
@@ -853,9 +866,10 @@
       <c r="C11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
         <v>45594</v>
       </c>
       <c r="B12" t="s">
@@ -864,9 +878,10 @@
       <c r="C12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
         <v>45601</v>
       </c>
       <c r="B13" t="s">
@@ -875,9 +890,10 @@
       <c r="C13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
         <v>45608</v>
       </c>
       <c r="B14" t="s">
@@ -886,9 +902,10 @@
       <c r="C14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
         <v>45615</v>
       </c>
       <c r="B15" t="s">
@@ -897,9 +914,10 @@
       <c r="C15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
         <v>45622</v>
       </c>
       <c r="B16" t="s">
@@ -908,9 +926,10 @@
       <c r="C16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
         <v>45629</v>
       </c>
       <c r="B17" t="s">
@@ -919,6 +938,7 @@
       <c r="C17" t="s">
         <v>8</v>
       </c>
+      <c r="G17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -929,7 +949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB6305A-7A3D-E944-958B-BA084CA13D72}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
First pass update for 2025
</commit_message>
<xml_diff>
--- a/files/schedule_modules.xlsx
+++ b/files/schedule_modules.xlsx
@@ -5,19 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu-my.sharepoint.com/personal/cooperstone_1_osu_edu/Documents/BuckeyeBox Data/JLC_Files/OSU/teaching/data-viz/rdataviz/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicacooperstone/Documents/git/rdataviz/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="13_ncr:1_{7C40CE6C-DF63-484C-A234-8A007B7633E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DADFFC60-5773-D145-B141-C181D957E330}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A5F6CC-1467-AC44-B3DD-EF4C9F98F11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13060" yWindow="3680" windowWidth="28800" windowHeight="16360" activeTab="1" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
+    <workbookView xWindow="22400" yWindow="3380" windowWidth="28800" windowHeight="16360" activeTab="1" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="2" r:id="rId1"/>
-    <sheet name="Schedule_date_2024" sheetId="5" r:id="rId2"/>
-    <sheet name="module_due_dates_2024" sheetId="6" r:id="rId3"/>
-    <sheet name="Schedule_date_2023" sheetId="3" r:id="rId4"/>
-    <sheet name="module_due_dates_2023" sheetId="4" r:id="rId5"/>
+    <sheet name="Schedule_date_2025" sheetId="7" r:id="rId2"/>
+    <sheet name="module_due_dates_2025" sheetId="8" r:id="rId3"/>
+    <sheet name="Schedule_date_2024" sheetId="5" r:id="rId4"/>
+    <sheet name="module_due_dates_2024" sheetId="6" r:id="rId5"/>
+    <sheet name="Schedule_date_2023" sheetId="3" r:id="rId6"/>
+    <sheet name="module_due_dates_2023" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="57">
   <si>
     <t>Principles of data visualization</t>
   </si>
@@ -163,6 +165,54 @@
   </si>
   <si>
     <t>Tuesday, October 29, 2024</t>
+  </si>
+  <si>
+    <t>Monday, September 1, 2025</t>
+  </si>
+  <si>
+    <t>Recitations</t>
+  </si>
+  <si>
+    <t>Sunday after each class</t>
+  </si>
+  <si>
+    <t>Tuesday, October 7, 2025</t>
+  </si>
+  <si>
+    <t>Tuesday, November 4, 2025</t>
+  </si>
+  <si>
+    <t>Tuesday, October 28, 2025</t>
+  </si>
+  <si>
+    <t>ggplot extension packages</t>
+  </si>
+  <si>
+    <t>Tuesday, December 9, 2025</t>
+  </si>
+  <si>
+    <t>Friday, December 12, 2025</t>
+  </si>
+  <si>
+    <t>No class, Veterans Day</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>4: Putting it together (asynchronous)</t>
+  </si>
+  <si>
+    <t>Capstone prep</t>
+  </si>
+  <si>
+    <t>Capstone plan prep, open session</t>
+  </si>
+  <si>
+    <t>Capstone assignment, open session</t>
+  </si>
+  <si>
+    <t>Manhattan plots and making lots of plots at once (asynchronous)</t>
   </si>
 </sst>
 </file>
@@ -170,7 +220,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -201,11 +251,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,7 +575,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,7 +635,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -594,7 +646,7 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -602,10 +654,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -616,7 +668,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -624,10 +676,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -635,10 +687,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -646,10 +698,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -660,7 +712,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -668,10 +720,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
+        <v>50</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -682,7 +734,7 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -690,10 +742,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -704,7 +756,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -724,10 +776,324 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D2FBAB-5424-1A47-B52E-30F77FDEB3FC}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>45895</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>45902</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>45909</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>45916</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>45923</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>45930</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>45937</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>45944</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>45951</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>45958</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>45965</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>45972</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>45979</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>45986</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>45993</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>46000</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07222E7-34D9-A648-B0D9-7893E36781B6}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E7002E-0E54-7A4A-93D0-B7490C5E682B}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
@@ -945,7 +1311,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB6305A-7A3D-E944-958B-BA084CA13D72}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1029,7 +1395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AC0B77-377C-2E43-B142-D9BC271E0496}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -1235,7 +1601,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48504950-6619-024D-BFE6-3D795EC0E695}">
   <dimension ref="A1:B7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Adjusting due dates, reordering content
</commit_message>
<xml_diff>
--- a/files/schedule_modules.xlsx
+++ b/files/schedule_modules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicacooperstone/Documents/git/rdataviz/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A5F6CC-1467-AC44-B3DD-EF4C9F98F11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74168391-F080-FB42-B2D3-842DE9D8D2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="3380" windowWidth="28800" windowHeight="16360" activeTab="1" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
+    <workbookView xWindow="22400" yWindow="2540" windowWidth="28800" windowHeight="16360" activeTab="1" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="2" r:id="rId1"/>
@@ -251,13 +251,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -933,7 +932,7 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
+      <c r="A13" s="3">
         <v>45972</v>
       </c>
       <c r="B13" t="s">
@@ -1002,7 +1001,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>